<commit_message>
removing unecessary files, and updatng collective
</commit_message>
<xml_diff>
--- a/top_pay.xlsx
+++ b/top_pay.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,11 @@
           <t>Median Salary (National)</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Median Salary (City)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -479,9 +484,12 @@
       <c r="D2" t="n">
         <v>135850</v>
       </c>
-      <c r="E2" t="n">
-        <v>103500</v>
-      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>103500</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -502,9 +510,12 @@
       <c r="D3" t="n">
         <v>132400</v>
       </c>
-      <c r="E3" t="n">
-        <v>103500</v>
-      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>103500</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -525,9 +536,12 @@
       <c r="D4" t="n">
         <v>129210</v>
       </c>
-      <c r="E4" t="n">
-        <v>103500</v>
-      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>103500</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -548,9 +562,12 @@
       <c r="D5" t="n">
         <v>126810</v>
       </c>
-      <c r="E5" t="n">
-        <v>103500</v>
-      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>103500</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -571,9 +588,12 @@
       <c r="D6" t="n">
         <v>124030</v>
       </c>
-      <c r="E6" t="n">
-        <v>103500</v>
-      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>103500</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -594,9 +614,12 @@
       <c r="D7" t="n">
         <v>121970</v>
       </c>
-      <c r="E7" t="n">
-        <v>103500</v>
-      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>103500</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -617,9 +640,12 @@
       <c r="D8" t="n">
         <v>117730</v>
       </c>
-      <c r="E8" t="n">
-        <v>103500</v>
-      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>103500</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -640,9 +666,12 @@
       <c r="D9" t="n">
         <v>112330</v>
       </c>
-      <c r="E9" t="n">
-        <v>103500</v>
-      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>103500</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -663,9 +692,12 @@
       <c r="D10" t="n">
         <v>109240</v>
       </c>
-      <c r="E10" t="n">
-        <v>103500</v>
-      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>103500</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -686,9 +718,12 @@
       <c r="D11" t="n">
         <v>108310</v>
       </c>
-      <c r="E11" t="n">
-        <v>103500</v>
-      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>103500</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>